<commit_message>
Update README and Practical
</commit_message>
<xml_diff>
--- a/PopGenomicsAdaptation.SebastianERamosOnsins/Practical/table_results.xlsx
+++ b/PopGenomicsAdaptation.SebastianERamosOnsins/Practical/table_results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sramos/Documents/CV/Classes/PopGenomics_Adaptation_Course-2022/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sramos/Documents/CV/Classes/PopGenomics_Adaptation_Course-2022/PopGenomicsAdaptation.SebastianERamosOnsins/Practical/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5B4C04-3281-D440-B198-7F046B507405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B854D5F-F07D-624C-A422-C8CA4BD28C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="7260" windowWidth="30240" windowHeight="10600" xr2:uid="{22CD8A5B-674F-4841-A11F-1094D6C1F9F5}"/>
   </bookViews>
@@ -36,19 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
-  <si>
-    <t>FuLi</t>
-  </si>
-  <si>
-    <t>Watt</t>
-  </si>
-  <si>
-    <t>Taj</t>
-  </si>
-  <si>
-    <t>FW</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>tendency</t>
   </si>
@@ -63,51 +51,6 @@
   </si>
   <si>
     <t>    </t>
-  </si>
-  <si>
-    <t>SNMR0</t>
-  </si>
-  <si>
-    <t>SNMRh</t>
-  </si>
-  <si>
-    <t>SSR0</t>
-  </si>
-  <si>
-    <t>SSRh</t>
-  </si>
-  <si>
-    <t>SNM-RED</t>
-  </si>
-  <si>
-    <t>SNM-EXP</t>
-  </si>
-  <si>
-    <t>DELF</t>
-  </si>
-  <si>
-    <t>DELG</t>
-  </si>
-  <si>
-    <t>DEL-EXP</t>
-  </si>
-  <si>
-    <t>PSL-DELF</t>
-  </si>
-  <si>
-    <t>PSH-DELF</t>
-  </si>
-  <si>
-    <t>PSM-DELF</t>
-  </si>
-  <si>
-    <t>PSH</t>
-  </si>
-  <si>
-    <t>PSM</t>
-  </si>
-  <si>
-    <t>PSL</t>
   </si>
   <si>
     <t>model</t>
@@ -522,7 +465,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -548,69 +491,69 @@
     <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F2" s="8" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
       <c r="J2" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="P2" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="3" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="O3" s="3"/>
       <c r="P3" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="7" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="C5" s="1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -624,7 +567,7 @@
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -663,7 +606,7 @@
     </row>
     <row r="16" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -684,7 +627,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC396465-A8CF-A541-B49B-240FFDADFEBE}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="B1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E16"/>
@@ -692,277 +635,101 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="5">
-        <v>-6.8913632753788701E-2</v>
-      </c>
-      <c r="C2" s="5">
-        <v>-5.8886303732259559E-2</v>
-      </c>
-      <c r="D2" s="5">
-        <v>-1.6321282624034206E-2</v>
-      </c>
-      <c r="E2" s="5">
-        <v>3.4634210432699208E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="5">
-        <v>-0.2190209613543419</v>
-      </c>
-      <c r="C3" s="5">
-        <v>-3.4384057657517619E-2</v>
-      </c>
-      <c r="D3" s="5">
-        <v>-1.9726508528773001E-2</v>
-      </c>
-      <c r="E3" s="5">
-        <v>2.5265949414001843E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="5">
-        <v>-6.6731550813139417E-2</v>
-      </c>
-      <c r="C4" s="5">
-        <v>-3.9645152118593208E-2</v>
-      </c>
-      <c r="D4" s="5">
-        <v>-4.203544739300713E-2</v>
-      </c>
-      <c r="E4" s="5">
-        <v>2.5659244497753142E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="5">
-        <v>-0.19826218689571418</v>
-      </c>
-      <c r="C5" s="5">
-        <v>-0.10690892759560078</v>
-      </c>
-      <c r="D5" s="5">
-        <v>-0.13949415378158281</v>
-      </c>
-      <c r="E5" s="5">
-        <v>-2.5502926967626349E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="5">
-        <v>-0.11858626569524078</v>
-      </c>
-      <c r="C6" s="5">
-        <v>-0.14583278642545783</v>
-      </c>
-      <c r="D6" s="5">
-        <v>-0.11154531734727002</v>
-      </c>
-      <c r="E6" s="5">
-        <v>-0.25974944494353891</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="5">
-        <v>-8.2288674562805975E-2</v>
-      </c>
-      <c r="C7" s="5">
-        <v>1.0286544921095375E-2</v>
-      </c>
-      <c r="D7" s="5">
-        <v>6.9524294851515123E-2</v>
-      </c>
-      <c r="E7" s="5">
-        <v>8.1770247374234661E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="5">
-        <v>-1.9341764729339501</v>
-      </c>
-      <c r="C8" s="5">
-        <v>-0.96081779781834054</v>
-      </c>
-      <c r="D8" s="5">
-        <v>-0.47599968360672862</v>
-      </c>
-      <c r="E8" s="5">
-        <v>-2.2287923005974264E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="5">
-        <v>-1.389964603846106</v>
-      </c>
-      <c r="C9" s="5">
-        <v>-0.69497747195697346</v>
-      </c>
-      <c r="D9" s="5">
-        <v>-0.42189970135861787</v>
-      </c>
-      <c r="E9" s="5">
-        <v>-3.3656340779747884E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="5">
-        <v>-1.8383362492859332</v>
-      </c>
-      <c r="C10" s="5">
-        <v>-0.92374056165277585</v>
-      </c>
-      <c r="D10" s="5">
-        <v>-0.31138997058665407</v>
-      </c>
-      <c r="E10" s="5">
-        <v>0.22541767703624138</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="5">
-        <v>-1.9656531704783737</v>
-      </c>
-      <c r="C11" s="5">
-        <v>-0.80496596870250814</v>
-      </c>
-      <c r="D11" s="5">
-        <v>-0.37025540545067148</v>
-      </c>
-      <c r="E11" s="5">
-        <v>0.19269873584881791</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="5">
-        <v>-0.72690205677846254</v>
-      </c>
-      <c r="C12" s="5">
-        <v>-0.25612716285454584</v>
-      </c>
-      <c r="D12" s="5">
-        <v>-1.5985298642669843E-2</v>
-      </c>
-      <c r="E12" s="5">
-        <v>0.10877199438614327</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="5">
-        <v>-0.57518130539887191</v>
-      </c>
-      <c r="C13" s="5">
-        <v>-0.19934785048206072</v>
-      </c>
-      <c r="D13" s="5">
-        <v>-3.7224981947932667E-2</v>
-      </c>
-      <c r="E13" s="5">
-        <v>3.0121730500278776E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="5">
-        <v>0.55009281843097091</v>
-      </c>
-      <c r="C14" s="5">
-        <v>0.43897705832629108</v>
-      </c>
-      <c r="D14" s="5">
-        <v>0.40006362998526579</v>
-      </c>
-      <c r="E14" s="5">
-        <v>0.15381113603256535</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="5">
-        <v>0.32526366786701222</v>
-      </c>
-      <c r="C15" s="5">
-        <v>0.28004163054822828</v>
-      </c>
-      <c r="D15" s="5">
-        <v>0.27235489869548368</v>
-      </c>
-      <c r="E15" s="5">
-        <v>6.1392976953104861E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="5">
-        <v>0.19438263386244359</v>
-      </c>
-      <c r="C16" s="5">
-        <v>0.1879521024320332</v>
-      </c>
-      <c r="D16" s="5">
-        <v>0.17946680623156364</v>
-      </c>
-      <c r="E16" s="5">
-        <v>6.1149672645152364E-2</v>
-      </c>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>